<commit_message>
fix bag in task 2|3
</commit_message>
<xml_diff>
--- a/user.xlsx
+++ b/user.xlsx
@@ -1,43 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,82 +50,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,95 +352,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="20.42578125" customWidth="1" min="1" max="1"/>
-    <col width="23.42578125" customWidth="1" min="2" max="2"/>
-    <col width="36" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Mail</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tema</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>tema@gmail.com</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>